<commit_message>
calorimetry : scripts : tests : updated
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.11.1.overfilled/data.xlsx
+++ b/input/calorimetry/ds.11.1.overfilled/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,6 @@
     <sheet name="heats" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="enthalpies" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="setup" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="tmp" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t xml:space="preserve">PRZ</t>
   </si>
@@ -86,9 +85,6 @@
   </si>
   <si>
     <t xml:space="preserve">constants </t>
-  </si>
-  <si>
-    <t xml:space="preserve">base concentrations</t>
   </si>
 </sst>
 </file>
@@ -626,7 +622,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1142,7 +1138,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1192,702 +1188,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K27"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="22.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="9.14"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>0.0001634</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>0.0001634</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>5.68309614333761E-006</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A2,4)</f>
-        <v>5.683E-006</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <f aca="false">D1*(1-heats!B4/setup!$B$2)+heats!B4*$G$2</f>
-        <v>5.6E-005</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">E1*(1-heats!B4/setup!$B$2)</f>
-        <v>0.000161732653061224</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <f aca="false">input_concentrations!A4/heats!B2</f>
-        <v>0.0056</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <f aca="false">input_concentrations!B3/setup!B2</f>
-        <v>0.000166734693877551</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <f aca="false">J1*(1-heats!B4/setup!$B$2)+heats!B4*$G$5</f>
-        <v>5.6E-005</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <f aca="false">K1*(1-heats!B4/setup!$B$2)</f>
-        <v>0.000161732653061224</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0.000151270019437322</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A3,4)</f>
-        <v>0.0001513</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <f aca="false">D2*(1-heats!B5/setup!$B$2)+heats!B5*$G$2</f>
-        <v>0.000111428571428571</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <f aca="false">E2*(1-heats!B5/setup!$B$2)</f>
-        <v>0.000160082319866722</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="false">J2*(1-heats!B5/setup!$B$2)+heats!B5*$G$5</f>
-        <v>0.000111428571428571</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <f aca="false">K2*(1-heats!B5/setup!$B$2)</f>
-        <v>0.000160082319866722</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.000164174243954135</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A4,4)</f>
-        <v>0.0001642</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <f aca="false">D3*(1-heats!B4/setup!$B$2)+heats!B4*$G$2</f>
-        <v>0.000166291545189504</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <f aca="false">E3*(1-heats!B4/setup!$B$2)</f>
-        <v>0.000158448826806858</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0.005488</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <f aca="false">J3*(1-heats!B4/setup!$B$2)+heats!B4*$G$5</f>
-        <v>0.000166291545189504</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <f aca="false">K3*(1-heats!B4/setup!$B$2)</f>
-        <v>0.000158448826806858</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>0.000161766685306602</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A5,4)</f>
-        <v>0.0001618</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <f aca="false">D4*(1-heats!B5/setup!$B$2)+heats!B5*$G$2</f>
-        <v>0.000220594692687571</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <f aca="false">E4*(1-heats!B5/setup!$B$2)</f>
-        <v>0.000156832002043522</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <f aca="false">G4/setup!$B$2</f>
-        <v>0.0056</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <f aca="false">J4*(1-heats!B5/setup!$B$2)+heats!B5*$G$5</f>
-        <v>0.000220594692687571</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <f aca="false">K4*(1-heats!B5/setup!$B$2)</f>
-        <v>0.000156832002043522</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0.000154410840917368</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A6,4)</f>
-        <v>0.0001544</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <f aca="false">D5*(1-heats!B6/setup!$B$2)+heats!B6*$G$2</f>
-        <v>0.000274343726435657</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <f aca="false">E5*(1-heats!B6/setup!$B$2)</f>
-        <v>0.000155231675492058</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <f aca="false">J5*(1-heats!B6/setup!$B$2)+heats!B6*$G$5</f>
-        <v>0.000274343726435657</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <f aca="false">K5*(1-heats!B6/setup!$B$2)</f>
-        <v>0.000155231675492058</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.000150812631382844</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A7,4)</f>
-        <v>0.0001508</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">D6*(1-heats!B7/setup!$B$2)+heats!B7*$G$2</f>
-        <v>0.000327544300655701</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <f aca="false">E6*(1-heats!B7/setup!$B$2)</f>
-        <v>0.000153647678803363</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="false">J6*(1-heats!B7/setup!$B$2)+heats!B7*$G$5</f>
-        <v>0.000327544300655701</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <f aca="false">K6*(1-heats!B7/setup!$B$2)</f>
-        <v>0.000153647678803363</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0.000147967580625029</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A8,4)</f>
-        <v>0.000148</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <f aca="false">D7*(1-heats!B8/setup!$B$2)+heats!B8*$G$2</f>
-        <v>0.0003802020118735</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <f aca="false">E7*(1-heats!B8/setup!$B$2)</f>
-        <v>0.000152079845346186</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <f aca="false">J7*(1-heats!B8/setup!$B$2)+heats!B8*$G$5</f>
-        <v>0.0003802020118735</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <f aca="false">K7*(1-heats!B8/setup!$B$2)</f>
-        <v>0.000152079845346186</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0.000142025213329922</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A9,4)</f>
-        <v>0.000142</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <f aca="false">D8*(1-heats!B9/setup!$B$2)+heats!B9*$G$2</f>
-        <v>0.000432322399507444</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <f aca="false">E8*(1-heats!B9/setup!$B$2)</f>
-        <v>0.000150528010189592</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <f aca="false">J8*(1-heats!B9/setup!$B$2)+heats!B9*$G$5</f>
-        <v>0.000432322399507444</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <f aca="false">K8*(1-heats!B9/setup!$B$2)</f>
-        <v>0.000150528010189592</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0.000140521924325731</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A10,4)</f>
-        <v>0.0001405</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <f aca="false">D9*(1-heats!B10/setup!$B$2)+heats!B10*$G$2</f>
-        <v>0.000483910946451245</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <f aca="false">E9*(1-heats!B10/setup!$B$2)</f>
-        <v>0.000148992010085617</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <f aca="false">J9*(1-heats!B10/setup!$B$2)+heats!B10*$G$5</f>
-        <v>0.000483910946451245</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <f aca="false">K9*(1-heats!B10/setup!$B$2)</f>
-        <v>0.000148992010085617</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>0.000138227683218485</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A11,4)</f>
-        <v>0.0001382</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <f aca="false">D10*(1-heats!B11/setup!$B$2)+heats!B11*$G$2</f>
-        <v>0.000534973079650723</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <f aca="false">E10*(1-heats!B11/setup!$B$2)</f>
-        <v>0.00014747168345209</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <f aca="false">J10*(1-heats!B11/setup!$B$2)+heats!B11*$G$5</f>
-        <v>0.000534973079650723</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <f aca="false">K10*(1-heats!B11/setup!$B$2)</f>
-        <v>0.00014747168345209</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>0.000134469100835544</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A12,4)</f>
-        <v>0.0001345</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <f aca="false">D11*(1-heats!B12/setup!$B$2)+heats!B12*$G$2</f>
-        <v>0.000585514170674695</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <f aca="false">E11*(1-heats!B12/setup!$B$2)</f>
-        <v>0.00014596687035564</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <f aca="false">J11*(1-heats!B12/setup!$B$2)+heats!B12*$G$5</f>
-        <v>0.000585514170674695</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">K11*(1-heats!B12/setup!$B$2)</f>
-        <v>0.00014596687035564</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>0.000131902338151592</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A13,4)</f>
-        <v>0.0001319</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <f aca="false">D12*(1-heats!B13/setup!$B$2)+heats!B13*$G$2</f>
-        <v>0.000635539536280055</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <f aca="false">E12*(1-heats!B13/setup!$B$2)</f>
-        <v>0.000144477412494869</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">J12*(1-heats!B13/setup!$B$2)+heats!B13*$G$5</f>
-        <v>0.000635539536280055</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">K12*(1-heats!B13/setup!$B$2)</f>
-        <v>0.000144477412494869</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>0.000129932017369441</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A14,4)</f>
-        <v>0.0001299</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <f aca="false">D13*(1-heats!B14/setup!$B$2)+heats!B14*$G$2</f>
-        <v>0.000685054438971075</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <f aca="false">E13*(1-heats!B14/setup!$B$2)</f>
-        <v>0.000143003153183696</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">J13*(1-heats!B14/setup!$B$2)+heats!B14*$G$5</f>
-        <v>0.000685054438971075</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">K13*(1-heats!B14/setup!$B$2)</f>
-        <v>0.000143003153183696</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>0.000125658951454205</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A15,4)</f>
-        <v>0.0001257</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <f aca="false">D14*(1-heats!B15/setup!$B$2)+heats!B15*$G$2</f>
-        <v>0.000734064087553003</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <f aca="false">E14*(1-heats!B15/setup!$B$2)</f>
-        <v>0.000141543937334883</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">J14*(1-heats!B15/setup!$B$2)+heats!B15*$G$5</f>
-        <v>0.000734064087553002</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">K14*(1-heats!B15/setup!$B$2)</f>
-        <v>0.000141543937334883</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>0.000121930716306095</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A16,4)</f>
-        <v>0.0001219</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <f aca="false">D15*(1-heats!B16/setup!$B$2)+heats!B16*$G$2</f>
-        <v>0.000782573637680013</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <f aca="false">E15*(1-heats!B16/setup!$B$2)</f>
-        <v>0.000140099611443711</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <f aca="false">J15*(1-heats!B16/setup!$B$2)+heats!B16*$G$5</f>
-        <v>0.000782573637680013</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">K15*(1-heats!B16/setup!$B$2)</f>
-        <v>0.000140099611443711</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>0.000119731498089042</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A17,4)</f>
-        <v>0.0001197</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <f aca="false">D16*(1-heats!B17/setup!$B$2)+heats!B17*$G$2</f>
-        <v>0.000830588192397564</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <f aca="false">E16*(1-heats!B17/setup!$B$2)</f>
-        <v>0.000138670023571836</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <f aca="false">J16*(1-heats!B17/setup!$B$2)+heats!B17*$G$5</f>
-        <v>0.000830588192397563</v>
-      </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">K16*(1-heats!B17/setup!$B$2)</f>
-        <v>0.000138670023571836</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>0.000116859819817852</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A18,4)</f>
-        <v>0.0001169</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <f aca="false">D17*(1-heats!B18/setup!$B$2)+heats!B18*$G$2</f>
-        <v>0.000878112802679221</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <f aca="false">E17*(1-heats!B18/setup!$B$2)</f>
-        <v>0.000137255023331307</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <f aca="false">J17*(1-heats!B18/setup!$B$2)+heats!B18*$G$5</f>
-        <v>0.000878112802679221</v>
-      </c>
-      <c r="K18" s="0" t="n">
-        <f aca="false">K17*(1-heats!B18/setup!$B$2)</f>
-        <v>0.000137255023331307</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>0.000113507286288302</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A19,4)</f>
-        <v>0.0001135</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <f aca="false">D18*(1-heats!B19/setup!$B$2)+heats!B19*$G$2</f>
-        <v>0.000925152467958004</v>
-      </c>
-      <c r="E19" s="0" t="n">
-        <f aca="false">E18*(1-heats!B19/setup!$B$2)</f>
-        <v>0.000135854461868743</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <f aca="false">J18*(1-heats!B19/setup!$B$2)+heats!B19*$G$5</f>
-        <v>0.000925152467958004</v>
-      </c>
-      <c r="K19" s="0" t="n">
-        <f aca="false">K18*(1-heats!B19/setup!$B$2)</f>
-        <v>0.000135854461868743</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>0.000110154933531191</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A20,4)</f>
-        <v>0.0001102</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <f aca="false">D19*(1-heats!B20/setup!$B$2)+heats!B20*$G$2</f>
-        <v>0.000971712136652311</v>
-      </c>
-      <c r="E20" s="0" t="n">
-        <f aca="false">E19*(1-heats!B20/setup!$B$2)</f>
-        <v>0.000134468191849674</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <f aca="false">J19*(1-heats!B20/setup!$B$2)+heats!B20*$G$5</f>
-        <v>0.00097171213665231</v>
-      </c>
-      <c r="K20" s="0" t="n">
-        <f aca="false">K19*(1-heats!B20/setup!$B$2)</f>
-        <v>0.000134468191849674</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>0.000109171976349646</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A21,4)</f>
-        <v>0.0001092</v>
-      </c>
-      <c r="D21" s="0" t="n">
-        <f aca="false">D20*(1-heats!B21/setup!$B$2)+heats!B21*$G$2</f>
-        <v>0.00101779670668647</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <f aca="false">E20*(1-heats!B21/setup!$B$2)</f>
-        <v>0.000133096067443045</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <f aca="false">J20*(1-heats!B21/setup!$B$2)+heats!B21*$G$5</f>
-        <v>0.00101779670668647</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <f aca="false">K20*(1-heats!B21/setup!$B$2)</f>
-        <v>0.000133096067443045</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>0.000104884426597035</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A22,4)</f>
-        <v>0.0001049</v>
-      </c>
-      <c r="D22" s="0" t="n">
-        <f aca="false">D21*(1-heats!B22/setup!$B$2)+heats!B22*$G$2</f>
-        <v>0.001063411026006</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <f aca="false">E21*(1-heats!B22/setup!$B$2)</f>
-        <v>0.000131737944305871</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <f aca="false">J21*(1-heats!B22/setup!$B$2)+heats!B22*$G$5</f>
-        <v>0.001063411026006</v>
-      </c>
-      <c r="K22" s="0" t="n">
-        <f aca="false">K21*(1-heats!B22/setup!$B$2)</f>
-        <v>0.000131737944305871</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>0.000103335196973618</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A23,4)</f>
-        <v>0.0001033</v>
-      </c>
-      <c r="D23" s="0" t="n">
-        <f aca="false">D22*(1-heats!B23/setup!$B$2)+heats!B23*$G$2</f>
-        <v>0.00110855989308757</v>
-      </c>
-      <c r="E23" s="0" t="n">
-        <f aca="false">E22*(1-heats!B23/setup!$B$2)</f>
-        <v>0.000130393679568056</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <f aca="false">J22*(1-heats!B23/setup!$B$2)+heats!B23*$G$5</f>
-        <v>0.00110855989308757</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <f aca="false">K22*(1-heats!B23/setup!$B$2)</f>
-        <v>0.000130393679568056</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>0.00010013899930567</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A24,4)</f>
-        <v>0.0001001</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <f aca="false">D23*(1-heats!B24/setup!$B$2)+heats!B24*$G$2</f>
-        <v>0.00115324805744382</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <f aca="false">E23*(1-heats!B24/setup!$B$2)</f>
-        <v>0.000129063131817361</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <f aca="false">J23*(1-heats!B24/setup!$B$2)+heats!B24*$G$5</f>
-        <v>0.00115324805744382</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <f aca="false">K23*(1-heats!B24/setup!$B$2)</f>
-        <v>0.000129063131817361</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>9.76601326246162E-005</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A25,4)</f>
-        <v>9.766E-005</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <f aca="false">D24*(1-heats!B25/setup!$B$2)+heats!B25*$G$2</f>
-        <v>0.00119748022012296</v>
-      </c>
-      <c r="E25" s="0" t="n">
-        <f aca="false">E24*(1-heats!B25/setup!$B$2)</f>
-        <v>0.000127746161084531</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <f aca="false">J24*(1-heats!B25/setup!$B$2)+heats!B25*$G$5</f>
-        <v>0.00119748022012296</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <f aca="false">K24*(1-heats!B25/setup!$B$2)</f>
-        <v>0.000127746161084531</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>9.32732611303209E-005</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <f aca="false">_xlfn.ORG.LIBREOFFICE.ROUNDSIG(A26,4)</f>
-        <v>9.327E-005</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <f aca="false">D25*(1-heats!B26/setup!$B$2)+heats!B26*$G$2</f>
-        <v>0.00124126103420334</v>
-      </c>
-      <c r="E26" s="0" t="n">
-        <f aca="false">E25*(1-heats!B26/setup!$B$2)</f>
-        <v>0.000126442628828567</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <f aca="false">J25*(1-heats!B26/setup!$B$2)+heats!B26*$G$5</f>
-        <v>0.00124126103420334</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <f aca="false">K25*(1-heats!B26/setup!$B$2)</f>
-        <v>0.000126442628828567</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>